<commit_message>
solutions excel class 3
</commit_message>
<xml_diff>
--- a/CLASS_B/01-Excel/3/Activities/03-Stu_LineAndBar/Unsolved/StudentGrades_Unsolved.xlsx
+++ b/CLASS_B/01-Excel/3/Activities/03-Stu_LineAndBar/Unsolved/StudentGrades_Unsolved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcorless/Documents/coding-boot-camp/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/3/Activities/03-Stu_LineAndBar/Unsolved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\datan\new\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\3\Activities\03-Stu_LineAndBar\Unsolved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF11C6CF-7FE8-144E-A1A7-5A6B159B58F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42597011-E775-4C07-942D-1B75EF4E6680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="14080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Tad Ethridge</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Jun</t>
+  </si>
+  <si>
+    <t>student</t>
   </si>
 </sst>
 </file>
@@ -461,16 +464,19 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="12" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
@@ -490,7 +496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +524,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -546,7 +552,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -574,7 +580,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -602,7 +608,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,7 +636,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -658,7 +664,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -686,7 +692,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -714,7 +720,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -742,7 +748,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -770,7 +776,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -798,7 +804,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -826,7 +832,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -854,7 +860,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -882,7 +888,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -910,7 +916,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -938,7 +944,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -966,7 +972,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -994,7 +1000,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1022,7 +1028,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>